<commit_message>
Adding fog gauge button to app
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/zl6_moved_instruments.xlsx
+++ b/Microclimate_data_supporting/zl6_moved_instruments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{2433BDE4-09BC-4FC2-9873-385C66F0ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFA0E4DC-5BD3-409E-9AB2-E43CE70402F2}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{2433BDE4-09BC-4FC2-9873-385C66F0ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C661AB7A-E1C8-4C00-B856-A895CE022512}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{387165D7-83F3-45DB-9650-B67354A4542D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Tree</t>
   </si>
@@ -84,6 +84,33 @@
   </si>
   <si>
     <t>ET6</t>
+  </si>
+  <si>
+    <t>TV4</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>PYR</t>
+  </si>
+  <si>
+    <t>Port.old</t>
+  </si>
+  <si>
+    <t>Port.new</t>
+  </si>
+  <si>
+    <t>FB8</t>
+  </si>
+  <si>
+    <t>Port 5 went bad</t>
+  </si>
+  <si>
+    <t>Port went bad</t>
   </si>
 </sst>
 </file>
@@ -456,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5684FF2-788A-4EA8-80B1-481E6A2E3499}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,11 +495,13 @@
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,13 +515,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -505,14 +543,14 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>45281</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -525,14 +563,14 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>45294</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -545,11 +583,98 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>45309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45314</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45314</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45315</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
May 2024 data upload
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/zl6_moved_instruments.xlsx
+++ b/Microclimate_data_supporting/zl6_moved_instruments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaug8\OneDrive - University of Kentucky\TMCF\Continuous_data\TMCF_Microclimate\Microclimate_data_supporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{2433BDE4-09BC-4FC2-9873-385C66F0ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C661AB7A-E1C8-4C00-B856-A895CE022512}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479CB254-7BA4-46E5-95D1-F8CA752AF120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{387165D7-83F3-45DB-9650-B67354A4542D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{387165D7-83F3-45DB-9650-B67354A4542D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Tree</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Port went bad</t>
+  </si>
+  <si>
+    <t>Removed datalogger</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,11 +546,17 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1">
         <v>45281</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -569,6 +578,9 @@
       <c r="H3" s="1">
         <v>45294</v>
       </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -583,11 +595,20 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
       <c r="H4" s="1">
         <v>45309</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
App update July 2024
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/zl6_moved_instruments.xlsx
+++ b/Microclimate_data_supporting/zl6_moved_instruments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaug8\OneDrive - University of Kentucky\TMCF\Continuous_data\TMCF_Microclimate\Microclimate_data_supporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479CB254-7BA4-46E5-95D1-F8CA752AF120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{479CB254-7BA4-46E5-95D1-F8CA752AF120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D02849FE-FC54-4702-8D51-892B03101CB0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{387165D7-83F3-45DB-9650-B67354A4542D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{387165D7-83F3-45DB-9650-B67354A4542D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>Tree</t>
   </si>
@@ -486,25 +486,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5684FF2-788A-4EA8-80B1-481E6A2E3499}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -559,7 +559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -611,7 +611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -640,7 +640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -669,7 +669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -696,6 +696,35 @@
       </c>
       <c r="I7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45401</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>